<commit_message>
variant 8 answers checke
</commit_message>
<xml_diff>
--- a/ЕГЭ/Варианты/2024/Вариант 8/files/18.xlsx
+++ b/ЕГЭ/Варианты/2024/Вариант 8/files/18.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\school\ЕГЭ\Варианты\2024\Вариант 8\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="18195" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="18" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -515,48 +520,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -564,14 +569,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -609,9 +617,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -646,7 +654,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -681,7 +689,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -855,9 +863,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1279,7 +1289,558 @@
         <v>93</v>
       </c>
     </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>MIN(SUM(A1, B15), SUM(A1, $A16))</f>
+        <v>-453</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:K15" si="0">MIN(SUM(B1, C15), SUM(B1, $A16))</f>
+        <v>-390</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>-335</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-283</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>-283</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>-247</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>-332</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>-236</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>-272</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>-224</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>-199</v>
+      </c>
+      <c r="L15">
+        <f>SUM(L1, $A16)</f>
+        <v>-156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" ref="A16:A24" si="1">MIN(SUM(A2, B16), SUM(A2, $A17))</f>
+        <v>-110</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ref="B16:B24" si="2">MIN(SUM(B2, C16), SUM(B2, $A17))</f>
+        <v>-148</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C24" si="3">MIN(SUM(C2, D16), SUM(C2, $A17))</f>
+        <v>-240</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D24" si="4">MIN(SUM(D2, E16), SUM(D2, $A17))</f>
+        <v>-178</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:E24" si="5">MIN(SUM(E2, F16), SUM(E2, $A17))</f>
+        <v>-232</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F24" si="6">MIN(SUM(F2, G16), SUM(F2, $A17))</f>
+        <v>-197</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G24" si="7">MIN(SUM(G2, H16), SUM(G2, $A17))</f>
+        <v>-213</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16:H24" si="8">MIN(SUM(H2, I16), SUM(H2, $A17))</f>
+        <v>-246</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ref="I16:I24" si="9">MIN(SUM(I2, J16), SUM(I2, $A17))</f>
+        <v>-129</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ref="J16:J24" si="10">MIN(SUM(J2, K16), SUM(J2, $A17))</f>
+        <v>-227</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ref="K16:K24" si="11">MIN(SUM(K2, L16), SUM(K2, $A17))</f>
+        <v>-272</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ref="L16:L24" si="12">SUM(L2, $A17)</f>
+        <v>-280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>-208</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>-131</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="3"/>
+        <v>-124</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="4"/>
+        <v>-143</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="5"/>
+        <v>-111</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="6"/>
+        <v>-154</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="7"/>
+        <v>-142</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="8"/>
+        <v>-225</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="9"/>
+        <v>-179</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="10"/>
+        <v>-162</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="11"/>
+        <v>-143</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="12"/>
+        <v>-186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>-110</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="2"/>
+        <v>-88</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="3"/>
+        <v>-70</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="4"/>
+        <v>-63</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="5"/>
+        <v>-92</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="6"/>
+        <v>-44</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="7"/>
+        <v>-44</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="9"/>
+        <v>-33</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="10"/>
+        <v>-129</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="11"/>
+        <v>-73</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="12"/>
+        <v>-66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>-64</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="3"/>
+        <v>111</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="5"/>
+        <v>61</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="6"/>
+        <v>74</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="7"/>
+        <v>135</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="8"/>
+        <v>61</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="9"/>
+        <v>101</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="10"/>
+        <v>78</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="11"/>
+        <v>82</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="12"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="2"/>
+        <v>311</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="3"/>
+        <v>251</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="4"/>
+        <v>157</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="5"/>
+        <v>264</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="6"/>
+        <v>231</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="7"/>
+        <v>299</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="8"/>
+        <v>294</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="9"/>
+        <v>281</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="10"/>
+        <v>262</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="11"/>
+        <v>254</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="12"/>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>218</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="2"/>
+        <v>194</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="4"/>
+        <v>195</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="5"/>
+        <v>184</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="6"/>
+        <v>88</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="7"/>
+        <v>152</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="8"/>
+        <v>248</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="9"/>
+        <v>160</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="10"/>
+        <v>222</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="11"/>
+        <v>125</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="12"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>187</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="3"/>
+        <v>279</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="4"/>
+        <v>238</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="5"/>
+        <v>281</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="6"/>
+        <v>240</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="7"/>
+        <v>338</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="8"/>
+        <v>260</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="9"/>
+        <v>256</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="10"/>
+        <v>289</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="11"/>
+        <v>312</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="12"/>
+        <v>357</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>338</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="2"/>
+        <v>252</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="3"/>
+        <v>198</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="4"/>
+        <v>163</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="6"/>
+        <v>193</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="7"/>
+        <v>122</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="8"/>
+        <v>106</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="9"/>
+        <v>124</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="10"/>
+        <v>193</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="11"/>
+        <v>256</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="12"/>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>329</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="2"/>
+        <v>251</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="3"/>
+        <v>263</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="4"/>
+        <v>299</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="5"/>
+        <v>277</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="6"/>
+        <v>252</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="7"/>
+        <v>248</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="8"/>
+        <v>307</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="9"/>
+        <v>312</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="10"/>
+        <v>296</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="11"/>
+        <v>428</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="12"/>
+        <v>369</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>SUM(A11, B25)</f>
+        <v>336</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ref="B25:L25" si="13">SUM(B11, C25)</f>
+        <v>313</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="13"/>
+        <v>283</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="13"/>
+        <v>293</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="13"/>
+        <v>204</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="13"/>
+        <v>109</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="13"/>
+        <v>89</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="13"/>
+        <v>48</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="13"/>
+        <v>99</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="13"/>
+        <v>41</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="13"/>
+        <v>44</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="13"/>
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
variant 8 23 solved
</commit_message>
<xml_diff>
--- a/ЕГЭ/Варианты/2024/Вариант 8/files/18.xlsx
+++ b/ЕГЭ/Варианты/2024/Вариант 8/files/18.xlsx
@@ -866,7 +866,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,498 +1291,498 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>MIN(SUM(A1, B15), SUM(A1, $A16))</f>
-        <v>-453</v>
+        <f>MAX(SUM(A1, B15), SUM(A1, $A16))</f>
+        <v>1751</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15:K15" si="0">MIN(SUM(B1, C15), SUM(B1, $A16))</f>
-        <v>-390</v>
+        <f t="shared" ref="B15:K15" si="0">MAX(SUM(B1, C15), SUM(B1, $A16))</f>
+        <v>1759</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>-335</v>
+        <v>1811</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>-283</v>
+        <v>1863</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>-283</v>
+        <v>1863</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>-247</v>
+        <v>1899</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>-332</v>
+        <v>1754</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>-236</v>
+        <v>1850</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>-272</v>
+        <v>1766</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>-224</v>
+        <v>1789</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>-199</v>
+        <v>1771</v>
       </c>
       <c r="L15">
         <f>SUM(L1, $A16)</f>
-        <v>-156</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" ref="A16:A24" si="1">MIN(SUM(A2, B16), SUM(A2, $A17))</f>
-        <v>-110</v>
+        <f t="shared" ref="A16:A24" si="1">MAX(SUM(A2, B16), SUM(A2, $A17))</f>
+        <v>1814</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:B24" si="2">MIN(SUM(B2, C16), SUM(B2, $A17))</f>
-        <v>-148</v>
+        <f t="shared" ref="B16:B24" si="2">MAX(SUM(B2, C16), SUM(B2, $A17))</f>
+        <v>1716</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:C24" si="3">MIN(SUM(C2, D16), SUM(C2, $A17))</f>
-        <v>-240</v>
+        <f t="shared" ref="C16:C24" si="3">MAX(SUM(C2, D16), SUM(C2, $A17))</f>
+        <v>1624</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16:D24" si="4">MIN(SUM(D2, E16), SUM(D2, $A17))</f>
-        <v>-178</v>
+        <f t="shared" ref="D16:D24" si="4">MAX(SUM(D2, E16), SUM(D2, $A17))</f>
+        <v>1656</v>
       </c>
       <c r="E16">
-        <f t="shared" ref="E16:E24" si="5">MIN(SUM(E2, F16), SUM(E2, $A17))</f>
-        <v>-232</v>
+        <f t="shared" ref="E16:E24" si="5">MAX(SUM(E2, F16), SUM(E2, $A17))</f>
+        <v>1602</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F24" si="6">MIN(SUM(F2, G16), SUM(F2, $A17))</f>
-        <v>-197</v>
+        <f t="shared" ref="F16:F24" si="6">MAX(SUM(F2, G16), SUM(F2, $A17))</f>
+        <v>1626</v>
       </c>
       <c r="G16">
-        <f t="shared" ref="G16:G24" si="7">MIN(SUM(G2, H16), SUM(G2, $A17))</f>
-        <v>-213</v>
+        <f t="shared" ref="G16:G24" si="7">MAX(SUM(G2, H16), SUM(G2, $A17))</f>
+        <v>1610</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:H24" si="8">MIN(SUM(H2, I16), SUM(H2, $A17))</f>
-        <v>-246</v>
+        <f t="shared" ref="H16:H24" si="8">MAX(SUM(H2, I16), SUM(H2, $A17))</f>
+        <v>1577</v>
       </c>
       <c r="I16">
-        <f t="shared" ref="I16:I24" si="9">MIN(SUM(I2, J16), SUM(I2, $A17))</f>
-        <v>-129</v>
+        <f t="shared" ref="I16:I24" si="9">MAX(SUM(I2, J16), SUM(I2, $A17))</f>
+        <v>1615</v>
       </c>
       <c r="J16">
-        <f t="shared" ref="J16:J24" si="10">MIN(SUM(J2, K16), SUM(J2, $A17))</f>
-        <v>-227</v>
+        <f t="shared" ref="J16:J24" si="10">MAX(SUM(J2, K16), SUM(J2, $A17))</f>
+        <v>1517</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:K24" si="11">MIN(SUM(K2, L16), SUM(K2, $A17))</f>
-        <v>-272</v>
+        <f t="shared" ref="K16:K24" si="11">MAX(SUM(K2, L16), SUM(K2, $A17))</f>
+        <v>1472</v>
       </c>
       <c r="L16">
         <f t="shared" ref="L16:L24" si="12">SUM(L2, $A17)</f>
-        <v>-280</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="1"/>
-        <v>-208</v>
+        <v>1464</v>
       </c>
       <c r="B17">
         <f t="shared" si="2"/>
-        <v>-131</v>
+        <v>1541</v>
       </c>
       <c r="C17">
         <f t="shared" si="3"/>
-        <v>-124</v>
+        <v>1548</v>
       </c>
       <c r="D17">
         <f t="shared" si="4"/>
-        <v>-143</v>
+        <v>1529</v>
       </c>
       <c r="E17">
         <f t="shared" si="5"/>
-        <v>-111</v>
+        <v>1561</v>
       </c>
       <c r="F17">
         <f t="shared" si="6"/>
-        <v>-154</v>
+        <v>1518</v>
       </c>
       <c r="G17">
         <f t="shared" si="7"/>
-        <v>-142</v>
+        <v>1530</v>
       </c>
       <c r="H17">
         <f t="shared" si="8"/>
-        <v>-225</v>
+        <v>1408</v>
       </c>
       <c r="I17">
         <f t="shared" si="9"/>
-        <v>-179</v>
+        <v>1454</v>
       </c>
       <c r="J17">
         <f t="shared" si="10"/>
-        <v>-162</v>
+        <v>1471</v>
       </c>
       <c r="K17">
         <f t="shared" si="11"/>
-        <v>-143</v>
+        <v>1490</v>
       </c>
       <c r="L17">
         <f t="shared" si="12"/>
-        <v>-186</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="1"/>
-        <v>-110</v>
+        <v>1447</v>
       </c>
       <c r="B18">
         <f t="shared" si="2"/>
-        <v>-88</v>
+        <v>1469</v>
       </c>
       <c r="C18">
         <f t="shared" si="3"/>
-        <v>-70</v>
+        <v>1487</v>
       </c>
       <c r="D18">
         <f t="shared" si="4"/>
-        <v>-63</v>
+        <v>1493</v>
       </c>
       <c r="E18">
         <f t="shared" si="5"/>
-        <v>-92</v>
+        <v>1464</v>
       </c>
       <c r="F18">
         <f t="shared" si="6"/>
-        <v>-44</v>
+        <v>1492</v>
       </c>
       <c r="G18">
         <f t="shared" si="7"/>
-        <v>-44</v>
+        <v>1472</v>
       </c>
       <c r="H18">
         <f t="shared" si="8"/>
-        <v>-12</v>
+        <v>1452</v>
       </c>
       <c r="I18">
         <f t="shared" si="9"/>
-        <v>-33</v>
+        <v>1400</v>
       </c>
       <c r="J18">
         <f t="shared" si="10"/>
-        <v>-129</v>
+        <v>1248</v>
       </c>
       <c r="K18">
         <f t="shared" si="11"/>
-        <v>-73</v>
+        <v>1297</v>
       </c>
       <c r="L18">
         <f t="shared" si="12"/>
-        <v>-66</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="1"/>
-        <v>-64</v>
+        <v>1304</v>
       </c>
       <c r="B19">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>1395</v>
       </c>
       <c r="C19">
         <f t="shared" si="3"/>
-        <v>111</v>
+        <v>1470</v>
       </c>
       <c r="D19">
         <f t="shared" si="4"/>
-        <v>99</v>
+        <v>1458</v>
       </c>
       <c r="E19">
         <f t="shared" si="5"/>
-        <v>61</v>
+        <v>1420</v>
       </c>
       <c r="F19">
         <f t="shared" si="6"/>
-        <v>74</v>
+        <v>1433</v>
       </c>
       <c r="G19">
         <f t="shared" si="7"/>
-        <v>135</v>
+        <v>1478</v>
       </c>
       <c r="H19">
         <f t="shared" si="8"/>
-        <v>61</v>
+        <v>1387</v>
       </c>
       <c r="I19">
         <f t="shared" si="9"/>
-        <v>101</v>
+        <v>1427</v>
       </c>
       <c r="J19">
         <f t="shared" si="10"/>
-        <v>78</v>
+        <v>1400</v>
       </c>
       <c r="K19">
         <f t="shared" si="11"/>
-        <v>82</v>
+        <v>1401</v>
       </c>
       <c r="L19">
         <f t="shared" si="12"/>
-        <v>153</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>1404</v>
       </c>
       <c r="B20">
         <f t="shared" si="2"/>
-        <v>311</v>
+        <v>1503</v>
       </c>
       <c r="C20">
         <f t="shared" si="3"/>
-        <v>251</v>
+        <v>1410</v>
       </c>
       <c r="D20">
         <f t="shared" si="4"/>
-        <v>157</v>
+        <v>1316</v>
       </c>
       <c r="E20">
         <f t="shared" si="5"/>
-        <v>264</v>
+        <v>1377</v>
       </c>
       <c r="F20">
         <f t="shared" si="6"/>
-        <v>231</v>
+        <v>1331</v>
       </c>
       <c r="G20">
         <f t="shared" si="7"/>
-        <v>299</v>
+        <v>1318</v>
       </c>
       <c r="H20">
         <f t="shared" si="8"/>
-        <v>294</v>
+        <v>1237</v>
       </c>
       <c r="I20">
         <f t="shared" si="9"/>
-        <v>281</v>
+        <v>1161</v>
       </c>
       <c r="J20">
         <f t="shared" si="10"/>
-        <v>262</v>
+        <v>1098</v>
       </c>
       <c r="K20">
         <f t="shared" si="11"/>
-        <v>254</v>
+        <v>1054</v>
       </c>
       <c r="L20">
         <f t="shared" si="12"/>
-        <v>313</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="1"/>
-        <v>218</v>
+        <v>923</v>
       </c>
       <c r="B21">
         <f t="shared" si="2"/>
-        <v>194</v>
+        <v>892</v>
       </c>
       <c r="C21">
         <f t="shared" si="3"/>
-        <v>232</v>
+        <v>885</v>
       </c>
       <c r="D21">
         <f t="shared" si="4"/>
-        <v>195</v>
+        <v>840</v>
       </c>
       <c r="E21">
         <f t="shared" si="5"/>
-        <v>184</v>
+        <v>829</v>
       </c>
       <c r="F21">
         <f t="shared" si="6"/>
-        <v>88</v>
+        <v>733</v>
       </c>
       <c r="G21">
         <f t="shared" si="7"/>
-        <v>152</v>
+        <v>797</v>
       </c>
       <c r="H21">
         <f t="shared" si="8"/>
-        <v>248</v>
+        <v>832</v>
       </c>
       <c r="I21">
         <f t="shared" si="9"/>
-        <v>160</v>
+        <v>744</v>
       </c>
       <c r="J21">
         <f t="shared" si="10"/>
-        <v>222</v>
+        <v>771</v>
       </c>
       <c r="K21">
         <f t="shared" si="11"/>
-        <v>125</v>
+        <v>674</v>
       </c>
       <c r="L21">
         <f t="shared" si="12"/>
-        <v>92</v>
+        <v>546</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="1"/>
-        <v>187</v>
+        <v>641</v>
       </c>
       <c r="B22">
         <f t="shared" si="2"/>
-        <v>255</v>
+        <v>709</v>
       </c>
       <c r="C22">
         <f t="shared" si="3"/>
-        <v>279</v>
+        <v>733</v>
       </c>
       <c r="D22">
         <f t="shared" si="4"/>
-        <v>238</v>
+        <v>690</v>
       </c>
       <c r="E22">
         <f t="shared" si="5"/>
-        <v>281</v>
+        <v>733</v>
       </c>
       <c r="F22">
         <f t="shared" si="6"/>
-        <v>240</v>
+        <v>676</v>
       </c>
       <c r="G22">
         <f t="shared" si="7"/>
-        <v>338</v>
+        <v>774</v>
       </c>
       <c r="H22">
         <f t="shared" si="8"/>
-        <v>260</v>
+        <v>696</v>
       </c>
       <c r="I22">
         <f t="shared" si="9"/>
-        <v>256</v>
+        <v>659</v>
       </c>
       <c r="J22">
         <f t="shared" si="10"/>
-        <v>289</v>
+        <v>669</v>
       </c>
       <c r="K22">
         <f t="shared" si="11"/>
-        <v>312</v>
+        <v>685</v>
       </c>
       <c r="L22">
         <f t="shared" si="12"/>
-        <v>357</v>
+        <v>711</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="1"/>
-        <v>338</v>
+        <v>692</v>
       </c>
       <c r="B23">
         <f t="shared" si="2"/>
-        <v>252</v>
+        <v>606</v>
       </c>
       <c r="C23">
         <f t="shared" si="3"/>
-        <v>198</v>
+        <v>552</v>
       </c>
       <c r="D23">
         <f t="shared" si="4"/>
-        <v>163</v>
+        <v>517</v>
       </c>
       <c r="E23">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>448</v>
       </c>
       <c r="F23">
         <f t="shared" si="6"/>
-        <v>193</v>
+        <v>541</v>
       </c>
       <c r="G23">
         <f t="shared" si="7"/>
-        <v>122</v>
+        <v>470</v>
       </c>
       <c r="H23">
         <f t="shared" si="8"/>
-        <v>106</v>
+        <v>436</v>
       </c>
       <c r="I23">
         <f t="shared" si="9"/>
-        <v>124</v>
+        <v>385</v>
       </c>
       <c r="J23">
         <f t="shared" si="10"/>
-        <v>193</v>
+        <v>391</v>
       </c>
       <c r="K23">
         <f t="shared" si="11"/>
-        <v>256</v>
+        <v>426</v>
       </c>
       <c r="L23">
         <f t="shared" si="12"/>
-        <v>284</v>
+        <v>409</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="1"/>
-        <v>329</v>
+        <v>454</v>
       </c>
       <c r="B24">
         <f t="shared" si="2"/>
-        <v>251</v>
+        <v>376</v>
       </c>
       <c r="C24">
         <f t="shared" si="3"/>
-        <v>263</v>
+        <v>388</v>
       </c>
       <c r="D24">
         <f t="shared" si="4"/>
-        <v>299</v>
+        <v>424</v>
       </c>
       <c r="E24">
         <f t="shared" si="5"/>
-        <v>277</v>
+        <v>402</v>
       </c>
       <c r="F24">
         <f t="shared" si="6"/>
-        <v>252</v>
+        <v>377</v>
       </c>
       <c r="G24">
         <f t="shared" si="7"/>
-        <v>248</v>
+        <v>373</v>
       </c>
       <c r="H24">
         <f t="shared" si="8"/>
-        <v>307</v>
+        <v>432</v>
       </c>
       <c r="I24">
         <f t="shared" si="9"/>
-        <v>312</v>
+        <v>437</v>
       </c>
       <c r="J24">
         <f t="shared" si="10"/>
-        <v>296</v>
+        <v>421</v>
       </c>
       <c r="K24">
         <f t="shared" si="11"/>
-        <v>428</v>
+        <v>461</v>
       </c>
       <c r="L24">
         <f t="shared" si="12"/>

</xml_diff>